<commit_message>
Implemented seek_food and seek_water behaviors
</commit_message>
<xml_diff>
--- a/CreatureSim_Stats.xlsx
+++ b/CreatureSim_Stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,13 +476,13 @@
         <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>99</v>
+        <v>99.57142857142857</v>
       </c>
       <c r="E2" t="n">
-        <v>99</v>
+        <v>99.57142857142857</v>
       </c>
       <c r="F2" t="n">
-        <v>99</v>
+        <v>99.57142857142857</v>
       </c>
     </row>
     <row r="3">
@@ -496,13 +496,13 @@
         <v>50</v>
       </c>
       <c r="D3" t="n">
-        <v>97</v>
+        <v>98.53846153846153</v>
       </c>
       <c r="E3" t="n">
-        <v>97</v>
+        <v>98.53846153846153</v>
       </c>
       <c r="F3" t="n">
-        <v>97</v>
+        <v>98.53846153846153</v>
       </c>
     </row>
     <row r="4">
@@ -516,13 +516,13 @@
         <v>50</v>
       </c>
       <c r="D4" t="n">
-        <v>95</v>
+        <v>97.47368421052632</v>
       </c>
       <c r="E4" t="n">
-        <v>95</v>
+        <v>97.47368421052632</v>
       </c>
       <c r="F4" t="n">
-        <v>95</v>
+        <v>97.47368421052632</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +536,13 @@
         <v>50</v>
       </c>
       <c r="D5" t="n">
-        <v>93</v>
+        <v>96.33333333333333</v>
       </c>
       <c r="E5" t="n">
-        <v>93</v>
+        <v>96.33333333333333</v>
       </c>
       <c r="F5" t="n">
-        <v>93</v>
+        <v>96.33333333333333</v>
       </c>
     </row>
     <row r="6">
@@ -556,13 +556,793 @@
         <v>50</v>
       </c>
       <c r="D6" t="n">
+        <v>94.33333333333333</v>
+      </c>
+      <c r="E6" t="n">
+        <v>94.33333333333333</v>
+      </c>
+      <c r="F6" t="n">
+        <v>94.33333333333333</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" t="n">
+        <v>92.33333333333333</v>
+      </c>
+      <c r="E7" t="n">
+        <v>92.33333333333333</v>
+      </c>
+      <c r="F7" t="n">
+        <v>92.33333333333333</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" t="n">
+        <v>90.33333333333333</v>
+      </c>
+      <c r="E8" t="n">
+        <v>90.33333333333333</v>
+      </c>
+      <c r="F8" t="n">
+        <v>90.33333333333333</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50</v>
+      </c>
+      <c r="D9" t="n">
+        <v>88.33333333333333</v>
+      </c>
+      <c r="E9" t="n">
+        <v>88.33333333333333</v>
+      </c>
+      <c r="F9" t="n">
+        <v>88.33333333333333</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>50</v>
+      </c>
+      <c r="D10" t="n">
+        <v>86.33333333333333</v>
+      </c>
+      <c r="E10" t="n">
+        <v>86.33333333333333</v>
+      </c>
+      <c r="F10" t="n">
+        <v>86.33333333333333</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" t="n">
+        <v>84.33333333333333</v>
+      </c>
+      <c r="E11" t="n">
+        <v>84.33333333333333</v>
+      </c>
+      <c r="F11" t="n">
+        <v>84.33333333333333</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50</v>
+      </c>
+      <c r="D12" t="n">
+        <v>82.33333333333333</v>
+      </c>
+      <c r="E12" t="n">
+        <v>82.33333333333333</v>
+      </c>
+      <c r="F12" t="n">
+        <v>82.33333333333333</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>50</v>
+      </c>
+      <c r="D13" t="n">
+        <v>80.33333333333333</v>
+      </c>
+      <c r="E13" t="n">
+        <v>80.33333333333333</v>
+      </c>
+      <c r="F13" t="n">
+        <v>80.33333333333333</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>50</v>
+      </c>
+      <c r="D14" t="n">
+        <v>78.33333333333333</v>
+      </c>
+      <c r="E14" t="n">
+        <v>78.33333333333333</v>
+      </c>
+      <c r="F14" t="n">
+        <v>78.33333333333333</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>50</v>
+      </c>
+      <c r="D15" t="n">
+        <v>76.33333333333333</v>
+      </c>
+      <c r="E15" t="n">
+        <v>76.33333333333333</v>
+      </c>
+      <c r="F15" t="n">
+        <v>76.33333333333333</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" t="n">
+        <v>74.33333333333333</v>
+      </c>
+      <c r="E16" t="n">
+        <v>74.33333333333333</v>
+      </c>
+      <c r="F16" t="n">
+        <v>74.33333333333333</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>50</v>
+      </c>
+      <c r="D17" t="n">
+        <v>72.33333333333333</v>
+      </c>
+      <c r="E17" t="n">
+        <v>72.33333333333333</v>
+      </c>
+      <c r="F17" t="n">
+        <v>72.33333333333333</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>50</v>
+      </c>
+      <c r="D18" t="n">
+        <v>70.33333333333333</v>
+      </c>
+      <c r="E18" t="n">
+        <v>70.33333333333333</v>
+      </c>
+      <c r="F18" t="n">
+        <v>70.33333333333333</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>50</v>
+      </c>
+      <c r="D19" t="n">
+        <v>68.33333333333333</v>
+      </c>
+      <c r="E19" t="n">
+        <v>68.33333333333333</v>
+      </c>
+      <c r="F19" t="n">
+        <v>69.75</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>50</v>
+      </c>
+      <c r="D20" t="n">
+        <v>66.33333333333333</v>
+      </c>
+      <c r="E20" t="n">
+        <v>66.33333333333333</v>
+      </c>
+      <c r="F20" t="n">
+        <v>76.125</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>50</v>
+      </c>
+      <c r="D21" t="n">
+        <v>64.33333333333333</v>
+      </c>
+      <c r="E21" t="n">
+        <v>66.83333333333333</v>
+      </c>
+      <c r="F21" t="n">
+        <v>88.79166666666667</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>50</v>
+      </c>
+      <c r="D22" t="n">
+        <v>62.33333333333334</v>
+      </c>
+      <c r="E22" t="n">
+        <v>69.83333333333333</v>
+      </c>
+      <c r="F22" t="n">
         <v>91</v>
       </c>
-      <c r="E6" t="n">
-        <v>91</v>
-      </c>
-      <c r="F6" t="n">
-        <v>91</v>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>50</v>
+      </c>
+      <c r="D23" t="n">
+        <v>60.33333333333334</v>
+      </c>
+      <c r="E23" t="n">
+        <v>77.83333333333333</v>
+      </c>
+      <c r="F23" t="n">
+        <v>92.08333333333333</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>50</v>
+      </c>
+      <c r="D24" t="n">
+        <v>58.33333333333334</v>
+      </c>
+      <c r="E24" t="n">
+        <v>79.58333333333333</v>
+      </c>
+      <c r="F24" t="n">
+        <v>93.375</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>50</v>
+      </c>
+      <c r="D25" t="n">
+        <v>56.33333333333334</v>
+      </c>
+      <c r="E25" t="n">
+        <v>81.33333333333333</v>
+      </c>
+      <c r="F25" t="n">
+        <v>91.375</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>50</v>
+      </c>
+      <c r="D26" t="n">
+        <v>54.33333333333334</v>
+      </c>
+      <c r="E26" t="n">
+        <v>80.58333333333333</v>
+      </c>
+      <c r="F26" t="n">
+        <v>89.375</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>50</v>
+      </c>
+      <c r="D27" t="n">
+        <v>52.33333333333334</v>
+      </c>
+      <c r="E27" t="n">
+        <v>82.33333333333333</v>
+      </c>
+      <c r="F27" t="n">
+        <v>87.375</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>50</v>
+      </c>
+      <c r="D28" t="n">
+        <v>50.33333333333334</v>
+      </c>
+      <c r="E28" t="n">
+        <v>80.33333333333333</v>
+      </c>
+      <c r="F28" t="n">
+        <v>85.375</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>50</v>
+      </c>
+      <c r="D29" t="n">
+        <v>48.33333333333334</v>
+      </c>
+      <c r="E29" t="n">
+        <v>78.33333333333333</v>
+      </c>
+      <c r="F29" t="n">
+        <v>83.375</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>50</v>
+      </c>
+      <c r="D30" t="n">
+        <v>46.33333333333334</v>
+      </c>
+      <c r="E30" t="n">
+        <v>76.33333333333333</v>
+      </c>
+      <c r="F30" t="n">
+        <v>81.375</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>50</v>
+      </c>
+      <c r="D31" t="n">
+        <v>44.33333333333334</v>
+      </c>
+      <c r="E31" t="n">
+        <v>74.33333333333333</v>
+      </c>
+      <c r="F31" t="n">
+        <v>79.375</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>50</v>
+      </c>
+      <c r="D32" t="n">
+        <v>42.33333333333334</v>
+      </c>
+      <c r="E32" t="n">
+        <v>72.33333333333333</v>
+      </c>
+      <c r="F32" t="n">
+        <v>77.375</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>50</v>
+      </c>
+      <c r="D33" t="n">
+        <v>40.33333333333334</v>
+      </c>
+      <c r="E33" t="n">
+        <v>74.08333333333333</v>
+      </c>
+      <c r="F33" t="n">
+        <v>75.375</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>50</v>
+      </c>
+      <c r="D34" t="n">
+        <v>38.33333333333334</v>
+      </c>
+      <c r="E34" t="n">
+        <v>75.83333333333333</v>
+      </c>
+      <c r="F34" t="n">
+        <v>73.375</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>50</v>
+      </c>
+      <c r="D35" t="n">
+        <v>36.33333333333334</v>
+      </c>
+      <c r="E35" t="n">
+        <v>77.58333333333333</v>
+      </c>
+      <c r="F35" t="n">
+        <v>71.375</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>50</v>
+      </c>
+      <c r="D36" t="n">
+        <v>34.33333333333334</v>
+      </c>
+      <c r="E36" t="n">
+        <v>83.08333333333333</v>
+      </c>
+      <c r="F36" t="n">
+        <v>69.375</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>50</v>
+      </c>
+      <c r="D37" t="n">
+        <v>32.33333333333334</v>
+      </c>
+      <c r="E37" t="n">
+        <v>82.33333333333333</v>
+      </c>
+      <c r="F37" t="n">
+        <v>67.375</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>50</v>
+      </c>
+      <c r="D38" t="n">
+        <v>30.33333333333333</v>
+      </c>
+      <c r="E38" t="n">
+        <v>80.33333333333333</v>
+      </c>
+      <c r="F38" t="n">
+        <v>68.33333333333333</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>50</v>
+      </c>
+      <c r="D39" t="n">
+        <v>28.33333333333333</v>
+      </c>
+      <c r="E39" t="n">
+        <v>78.33333333333333</v>
+      </c>
+      <c r="F39" t="n">
+        <v>77.29166666666667</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" t="n">
+        <v>50</v>
+      </c>
+      <c r="D40" t="n">
+        <v>26.33333333333333</v>
+      </c>
+      <c r="E40" t="n">
+        <v>76.33333333333333</v>
+      </c>
+      <c r="F40" t="n">
+        <v>83.41666666666667</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" t="n">
+        <v>50</v>
+      </c>
+      <c r="D41" t="n">
+        <v>24.33333333333333</v>
+      </c>
+      <c r="E41" t="n">
+        <v>75.58333333333333</v>
+      </c>
+      <c r="F41" t="n">
+        <v>84.75</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" t="n">
+        <v>50</v>
+      </c>
+      <c r="D42" t="n">
+        <v>22.33333333333333</v>
+      </c>
+      <c r="E42" t="n">
+        <v>74.83333333333333</v>
+      </c>
+      <c r="F42" t="n">
+        <v>87.66666666666667</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" t="n">
+        <v>50</v>
+      </c>
+      <c r="D43" t="n">
+        <v>20.33333333333333</v>
+      </c>
+      <c r="E43" t="n">
+        <v>75.33333333333333</v>
+      </c>
+      <c r="F43" t="n">
+        <v>93.91666666666667</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" t="n">
+        <v>50</v>
+      </c>
+      <c r="D44" t="n">
+        <v>18.33333333333333</v>
+      </c>
+      <c r="E44" t="n">
+        <v>74.58333333333333</v>
+      </c>
+      <c r="F44" t="n">
+        <v>91.91666666666667</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" t="n">
+        <v>50</v>
+      </c>
+      <c r="D45" t="n">
+        <v>16.33333333333333</v>
+      </c>
+      <c r="E45" t="n">
+        <v>72.58333333333333</v>
+      </c>
+      <c r="F45" t="n">
+        <v>89.91666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>